<commit_message>
updated send feed back mail
</commit_message>
<xml_diff>
--- a/output/resume_db.xlsx
+++ b/output/resume_db.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G52"/>
+  <dimension ref="A1:G57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1999,6 +1999,161 @@
       </c>
       <c r="G52" t="inlineStr"/>
     </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>SANTOSH  KUMAR  DASH</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>Santoshkdash27@gmail.com</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>1 years</t>
+        </is>
+      </c>
+      <c r="E53" t="n">
+        <v>38.9</v>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>+91 8197576872</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr"/>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>Soumya Ranjan Swain</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>soumya18.swain@gmail.com</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>No Experience</t>
+        </is>
+      </c>
+      <c r="E54" t="n">
+        <v>43.02</v>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>+91-7077964867</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr"/>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>SANTOSH  KUMAR  DASH</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>Santoshkdash27@gmail.com</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>1 years</t>
+        </is>
+      </c>
+      <c r="E55" t="n">
+        <v>39.07</v>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>+91 8197576872</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr"/>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>Soumya Ranjan Swain</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>soumya18.swain@gmail.com</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>2023</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>No Experience</t>
+        </is>
+      </c>
+      <c r="E56" t="n">
+        <v>43.02</v>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>+91-7077964867</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr"/>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>Job Description</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>No Experience</t>
+        </is>
+      </c>
+      <c r="E57" t="n">
+        <v>100</v>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>